<commit_message>
sql RP_BR_GATHER_SUBPROC select 及matchid varchar(32)修改
</commit_message>
<xml_diff>
--- a/会鸽业务系统全景图/会鸽定位业务数据库表.xlsx
+++ b/会鸽业务系统全景图/会鸽定位业务数据库表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="总览表" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749">
   <si>
     <t>基础信息表</t>
   </si>
@@ -2218,6 +2218,30 @@
 2---业务</t>
   </si>
   <si>
+    <t>比赛成绩记录表</t>
+  </si>
+  <si>
+    <t>RP_BR_MATCH_RESULT</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>Number(8,3)</t>
+  </si>
+  <si>
+    <t>单位公里，小数点为3位</t>
+  </si>
+  <si>
+    <t>MINUTE_SPEED</t>
+  </si>
+  <si>
+    <t>分速</t>
+  </si>
+  <si>
+    <t>距离（以米为单位）除以时差(分钟为单位，秒按照小数计算)，保留小数点为4位；</t>
+  </si>
+  <si>
     <t>基础表
 1.与  的关联（）</t>
   </si>
@@ -2338,12 +2362,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -2361,105 +2385,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2481,9 +2409,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2500,6 +2448,82 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2550,7 +2574,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2562,7 +2628,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2574,49 +2664,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2628,7 +2676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2640,19 +2694,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2664,37 +2724,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2706,25 +2748,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2801,11 +2825,74 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2827,54 +2914,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2883,172 +2922,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3059,12 +3083,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3087,8 +3111,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4184,23 +4214,23 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="34" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4310,44 +4340,44 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32" t="s">
+      <c r="E19" s="34"/>
+      <c r="F19" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="34" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33" t="s">
+      <c r="E20" s="35"/>
+      <c r="F20" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="35" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4366,44 +4396,44 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32" t="s">
+      <c r="E22" s="34"/>
+      <c r="F22" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="34" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32" t="s">
+      <c r="E23" s="34"/>
+      <c r="F23" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="34" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4419,7 +4449,7 @@
   <sheetPr/>
   <dimension ref="A1:F302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+    <sheetView topLeftCell="A263" workbookViewId="0">
       <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
@@ -6065,7 +6095,7 @@
         <v>16</v>
       </c>
       <c r="E101" s="13"/>
-      <c r="F101" s="21" t="s">
+      <c r="F101" s="23" t="s">
         <v>282</v>
       </c>
     </row>
@@ -6352,7 +6382,7 @@
         <v>279</v>
       </c>
       <c r="D117" s="10"/>
-      <c r="E117" s="22">
+      <c r="E117" s="24">
         <v>42563</v>
       </c>
       <c r="F117" s="2"/>
@@ -7232,12 +7262,12 @@
       </c>
     </row>
     <row r="172" spans="1:6">
-      <c r="A172" s="23"/>
-      <c r="B172" s="23"/>
-      <c r="C172" s="23"/>
-      <c r="D172" s="23"/>
-      <c r="E172" s="24"/>
-      <c r="F172" s="23"/>
+      <c r="A172" s="25"/>
+      <c r="B172" s="25"/>
+      <c r="C172" s="25"/>
+      <c r="D172" s="25"/>
+      <c r="E172" s="26"/>
+      <c r="F172" s="25"/>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="2" t="s">
@@ -7758,20 +7788,20 @@
       </c>
     </row>
     <row r="204" spans="1:6">
-      <c r="A204" s="23"/>
-      <c r="B204" s="23"/>
-      <c r="C204" s="23"/>
-      <c r="D204" s="23"/>
-      <c r="E204" s="24"/>
-      <c r="F204" s="23"/>
+      <c r="A204" s="25"/>
+      <c r="B204" s="25"/>
+      <c r="C204" s="25"/>
+      <c r="D204" s="25"/>
+      <c r="E204" s="26"/>
+      <c r="F204" s="25"/>
     </row>
     <row r="205" spans="1:6">
-      <c r="A205" s="23"/>
-      <c r="B205" s="23"/>
-      <c r="C205" s="23"/>
-      <c r="D205" s="23"/>
-      <c r="E205" s="24"/>
-      <c r="F205" s="23"/>
+      <c r="A205" s="25"/>
+      <c r="B205" s="25"/>
+      <c r="C205" s="25"/>
+      <c r="D205" s="25"/>
+      <c r="E205" s="26"/>
+      <c r="F205" s="25"/>
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="2" t="s">
@@ -7920,7 +7950,7 @@
       <c r="D214" s="2">
         <v>16</v>
       </c>
-      <c r="E214" s="25">
+      <c r="E214" s="27">
         <v>13880081234</v>
       </c>
       <c r="F214" s="2"/>
@@ -8046,7 +8076,7 @@
         <v>369</v>
       </c>
       <c r="D221" s="10"/>
-      <c r="E221" s="22">
+      <c r="E221" s="24">
         <v>41091</v>
       </c>
       <c r="F221" s="2" t="s">
@@ -8054,48 +8084,48 @@
       </c>
     </row>
     <row r="222" spans="1:6">
-      <c r="A222" s="23"/>
-      <c r="B222" s="23"/>
-      <c r="C222" s="23"/>
-      <c r="D222" s="23"/>
-      <c r="E222" s="24"/>
-      <c r="F222" s="23"/>
+      <c r="A222" s="25"/>
+      <c r="B222" s="25"/>
+      <c r="C222" s="25"/>
+      <c r="D222" s="25"/>
+      <c r="E222" s="26"/>
+      <c r="F222" s="25"/>
     </row>
     <row r="224" spans="1:6">
       <c r="A224" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B224" s="26" t="s">
+      <c r="B224" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C224" s="27"/>
-      <c r="D224" s="27"/>
-      <c r="E224" s="27"/>
-      <c r="F224" s="28"/>
+      <c r="C224" s="29"/>
+      <c r="D224" s="29"/>
+      <c r="E224" s="29"/>
+      <c r="F224" s="30"/>
     </row>
     <row r="225" spans="1:6">
       <c r="A225" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B225" s="26" t="s">
+      <c r="B225" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C225" s="27"/>
-      <c r="D225" s="27"/>
-      <c r="E225" s="27"/>
-      <c r="F225" s="28"/>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29"/>
+      <c r="E225" s="29"/>
+      <c r="F225" s="30"/>
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B226" s="29" t="s">
+      <c r="B226" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="C226" s="30"/>
-      <c r="D226" s="30"/>
-      <c r="E226" s="30"/>
-      <c r="F226" s="31"/>
+      <c r="C226" s="32"/>
+      <c r="D226" s="32"/>
+      <c r="E226" s="32"/>
+      <c r="F226" s="33"/>
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="2" t="s">
@@ -8234,7 +8264,7 @@
       <c r="D234" s="7">
         <v>16</v>
       </c>
-      <c r="E234" s="25">
+      <c r="E234" s="27">
         <v>13880081234</v>
       </c>
       <c r="F234" s="2"/>
@@ -8612,12 +8642,12 @@
       </c>
     </row>
     <row r="256" spans="1:6">
-      <c r="A256" s="23"/>
-      <c r="B256" s="23"/>
-      <c r="C256" s="23"/>
-      <c r="D256" s="23"/>
-      <c r="E256" s="24"/>
-      <c r="F256" s="23"/>
+      <c r="A256" s="25"/>
+      <c r="B256" s="25"/>
+      <c r="C256" s="25"/>
+      <c r="D256" s="25"/>
+      <c r="E256" s="26"/>
+      <c r="F256" s="25"/>
     </row>
     <row r="258" spans="1:6">
       <c r="A258" s="2" t="s">
@@ -9196,7 +9226,7 @@
       <c r="D291" s="7">
         <v>16</v>
       </c>
-      <c r="E291" s="25">
+      <c r="E291" s="27">
         <v>13880081234</v>
       </c>
       <c r="F291" s="2"/>
@@ -9436,10 +9466,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F209"/>
+  <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="I218" sqref="I218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -9516,10 +9546,10 @@
         <v>360</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D5" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
@@ -10238,10 +10268,10 @@
         <v>360</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D50" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="2"/>
@@ -10745,10 +10775,10 @@
         <v>360</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D79" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="2"/>
@@ -11003,10 +11033,10 @@
         <v>360</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D97" s="2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="2"/>
@@ -11636,10 +11666,10 @@
         <v>360</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D136" s="19">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E136" s="18"/>
       <c r="F136" s="19"/>
@@ -12144,10 +12174,10 @@
         <v>360</v>
       </c>
       <c r="C166" s="19" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="D166" s="19">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="E166" s="18"/>
       <c r="F166" s="19" t="s">
@@ -12914,8 +12944,606 @@
       </c>
       <c r="F209" s="16"/>
     </row>
+    <row r="212" spans="1:6">
+      <c r="A212" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="C212" s="3"/>
+      <c r="D212" s="3"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="3"/>
+    </row>
+    <row r="213" spans="1:6">
+      <c r="A213" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C213" s="3"/>
+      <c r="D213" s="3"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="3"/>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
+      <c r="E214" s="5"/>
+      <c r="F214" s="5"/>
+    </row>
+    <row r="215" spans="1:6">
+      <c r="A215" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
+      <c r="A216" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D216" s="2">
+        <v>32</v>
+      </c>
+      <c r="E216" s="3"/>
+      <c r="F216" s="2"/>
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D217" s="2">
+        <v>256</v>
+      </c>
+      <c r="E217" s="3"/>
+      <c r="F217" s="2"/>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D218" s="2">
+        <v>16</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F218" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D219" s="2">
+        <v>32</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F219" s="2"/>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D220" s="2">
+        <v>32</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D221" s="10">
+        <v>16</v>
+      </c>
+      <c r="E221" s="3"/>
+      <c r="F221" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D222" s="2">
+        <v>32</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D223" s="2">
+        <v>256</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F223" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D224" s="2">
+        <v>10</v>
+      </c>
+      <c r="E224" s="3">
+        <v>104.022747</v>
+      </c>
+      <c r="F224" s="2"/>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D225" s="2">
+        <v>10</v>
+      </c>
+      <c r="E225" s="3">
+        <v>30.666549</v>
+      </c>
+      <c r="F225" s="2"/>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D226" s="2">
+        <v>16</v>
+      </c>
+      <c r="E226" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F226" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D227" s="2">
+        <v>1</v>
+      </c>
+      <c r="E227" s="6">
+        <v>1</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D228" s="2">
+        <v>1</v>
+      </c>
+      <c r="E228" s="6">
+        <v>1</v>
+      </c>
+      <c r="F228" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D229" s="2">
+        <v>1</v>
+      </c>
+      <c r="E229" s="6">
+        <v>1</v>
+      </c>
+      <c r="F229" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D230" s="2">
+        <v>16</v>
+      </c>
+      <c r="E230" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F230" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D231" s="2">
+        <v>16</v>
+      </c>
+      <c r="E231" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="F231" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D232" s="2">
+        <v>16</v>
+      </c>
+      <c r="E232" s="6"/>
+      <c r="F232" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="B233" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="C233" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="D233" s="16"/>
+      <c r="E233" s="21">
+        <v>42564.3333333333</v>
+      </c>
+      <c r="F233" s="2"/>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B234" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="C234" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D234" s="16">
+        <v>256</v>
+      </c>
+      <c r="E234" s="22"/>
+      <c r="F234" s="2"/>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="B235" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C235" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D235" s="16">
+        <v>10</v>
+      </c>
+      <c r="E235" s="22">
+        <v>104.022747</v>
+      </c>
+      <c r="F235" s="2"/>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B236" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="C236" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D236" s="16">
+        <v>10</v>
+      </c>
+      <c r="E236" s="22">
+        <v>30.666549</v>
+      </c>
+      <c r="F236" s="2"/>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D237" s="8">
+        <v>16</v>
+      </c>
+      <c r="E237" s="13"/>
+      <c r="F237" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="C238" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D238" s="8">
+        <v>16</v>
+      </c>
+      <c r="E238" s="13"/>
+      <c r="F238" s="8" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D239" s="8">
+        <v>10</v>
+      </c>
+      <c r="E239" s="13">
+        <v>104.022747</v>
+      </c>
+      <c r="F239" s="8" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="C240" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D240" s="8">
+        <v>10</v>
+      </c>
+      <c r="E240" s="13">
+        <v>30.666549</v>
+      </c>
+      <c r="F240" s="8"/>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D241" s="2">
+        <v>8</v>
+      </c>
+      <c r="E241" s="3">
+        <v>500</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="B242" s="10" t="s">
+        <v>652</v>
+      </c>
+      <c r="C242" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="D242" s="2"/>
+      <c r="E242" s="17">
+        <v>42564.3333333333</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="B243" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C243" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="D243" s="2">
+        <v>8</v>
+      </c>
+      <c r="E243" s="13">
+        <v>324.411</v>
+      </c>
+      <c r="F243" s="2" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="B244" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="C244" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="D244" s="2">
+        <v>8</v>
+      </c>
+      <c r="E244" s="13">
+        <v>607.7197</v>
+      </c>
+      <c r="F244" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
@@ -12937,6 +13565,9 @@
     <mergeCell ref="B197:F197"/>
     <mergeCell ref="B198:F198"/>
     <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300"/>
@@ -12992,7 +13623,7 @@
         <v>150</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -13041,7 +13672,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>704</v>
+        <v>712</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>267</v>
@@ -13059,7 +13690,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>270</v>
@@ -13075,7 +13706,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>272</v>
@@ -13109,7 +13740,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>276</v>
@@ -13127,10 +13758,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>709</v>
+        <v>717</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>220</v>
@@ -13142,15 +13773,15 @@
         <v>1800</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>710</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>711</v>
+        <v>719</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>220</v>
@@ -13162,15 +13793,15 @@
         <v>120</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>713</v>
+        <v>721</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>714</v>
+        <v>722</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>715</v>
+        <v>723</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>220</v>
@@ -13182,15 +13813,15 @@
         <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>279</v>
@@ -13199,16 +13830,16 @@
         <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>279</v>
@@ -13217,10 +13848,10 @@
         <v>16</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -13252,7 +13883,7 @@
         <v>150</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -13301,7 +13932,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>248</v>
@@ -13317,7 +13948,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>250</v>
@@ -13336,7 +13967,7 @@
         <v>173</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>723</v>
+        <v>731</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>158</v>
@@ -13351,10 +13982,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>724</v>
+        <v>732</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>158</v>
@@ -13369,10 +14000,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>279</v>
@@ -13381,7 +14012,7 @@
         <v>16</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -13402,7 +14033,7 @@
         <v>104.022747</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -13422,15 +14053,15 @@
         <v>30.666549</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>279</v>
@@ -13439,10 +14070,10 @@
         <v>16</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -13474,7 +14105,7 @@
         <v>150</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -13503,7 +14134,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>726</v>
+        <v>734</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>349</v>
@@ -13523,7 +14154,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>351</v>
@@ -13539,7 +14170,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>353</v>
@@ -13573,7 +14204,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>358</v>
@@ -13591,10 +14222,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>279</v>
@@ -13603,16 +14234,16 @@
         <v>16</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>279</v>
@@ -13621,10 +14252,10 @@
         <v>16</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -13656,7 +14287,7 @@
         <v>150</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -13705,10 +14336,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>727</v>
+        <v>735</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>158</v>
@@ -13724,7 +14355,7 @@
         <v>173</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>158</v>
@@ -13739,10 +14370,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>158</v>
@@ -13757,10 +14388,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>730</v>
+        <v>738</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>220</v>
@@ -13772,15 +14403,15 @@
         <v>30</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>732</v>
+        <v>740</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>220</v>
@@ -13792,15 +14423,15 @@
         <v>180</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>736</v>
+        <v>744</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>737</v>
+        <v>745</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>220</v>
@@ -13812,15 +14443,15 @@
         <v>60</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>738</v>
+        <v>746</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>279</v>
@@ -13829,16 +14460,16 @@
         <v>16</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>279</v>
@@ -13847,10 +14478,10 @@
         <v>16</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -13882,7 +14513,7 @@
         <v>150</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -13931,7 +14562,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>440</v>
@@ -13965,7 +14596,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>444</v>
@@ -13983,10 +14614,10 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>279</v>
@@ -13995,16 +14626,16 @@
         <v>16</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>279</v>
@@ -14013,10 +14644,10 @@
         <v>16</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -14048,7 +14679,7 @@
         <v>150</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -14077,10 +14708,10 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>739</v>
+        <v>747</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>158</v>
@@ -14169,10 +14800,10 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>279</v>
@@ -14181,16 +14812,16 @@
         <v>16</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>279</v>
@@ -14199,10 +14830,10 @@
         <v>16</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
   </sheetData>

</xml_diff>